<commit_message>
Test-7 tree (MSE, thisyear)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-7.xlsx
+++ b/migforecasting/underground/test-7.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="ThisYear" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="14">
   <si>
     <t>test size 20%</t>
   </si>
@@ -50,6 +50,18 @@
   </si>
   <si>
     <t>test (MSE)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (citiesdataset-2.csv) - this year</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (citiesdataset-DCor-3.csv) - this year</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (citiesdataset-NYDcor-2.csv) - this year</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (citiesdataset-NYDCor-3.csv) - this year</t>
   </si>
 </sst>
 </file>
@@ -395,12 +407,2275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C3:V58"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" customWidth="1"/>
+    <col min="17" max="17" width="17" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="O4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="T4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="V4" s="1"/>
+    </row>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.2056791044918189</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.2729879855922368</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.99227540458748931</v>
+      </c>
+      <c r="J6" s="3">
+        <v>3.8642212638417548</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1</v>
+      </c>
+      <c r="P6" s="4">
+        <v>9.2782693771926853E-4</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>7.4456010906704777E-3</v>
+      </c>
+      <c r="T6" s="2">
+        <v>1</v>
+      </c>
+      <c r="U6" s="4">
+        <v>9.1196311480614453E-4</v>
+      </c>
+      <c r="V6" s="4">
+        <v>5.8380202018514724E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <f>C6+1</f>
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.99795762614404582</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3.3400541455661759</v>
+      </c>
+      <c r="H7" s="2">
+        <f>H6+1</f>
+        <v>2</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1.143090497212109</v>
+      </c>
+      <c r="J7" s="3">
+        <v>3.5180831224252911</v>
+      </c>
+      <c r="O7" s="2">
+        <f>O6+1</f>
+        <v>2</v>
+      </c>
+      <c r="P7" s="4">
+        <v>9.7669092535360874E-4</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>6.4287108033408806E-3</v>
+      </c>
+      <c r="T7" s="2">
+        <f>T6+1</f>
+        <v>2</v>
+      </c>
+      <c r="U7" s="4">
+        <v>1.0022162063098019E-3</v>
+      </c>
+      <c r="V7" s="4">
+        <v>5.3046415388013123E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f t="shared" ref="C8:C55" si="0">C7+1</f>
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.13311698930376</v>
+      </c>
+      <c r="E8" s="3">
+        <v>4.4462560975719221</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" ref="H8:H55" si="1">H7+1</f>
+        <v>3</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1.279606043959526</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1.621863536133122</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" ref="O8:O55" si="2">O7+1</f>
+        <v>3</v>
+      </c>
+      <c r="P8" s="4">
+        <v>8.3292902858249167E-4</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>8.3401381509059652E-3</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" ref="T8:T55" si="3">T7+1</f>
+        <v>3</v>
+      </c>
+      <c r="U8" s="4">
+        <v>9.5276356433865287E-4</v>
+      </c>
+      <c r="V8" s="4">
+        <v>6.0639691734625956E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.125196249673893</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3.047146786999464</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1.418731042483161</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1.682368968146345</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="P9" s="4">
+        <v>9.2014789436484885E-4</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>6.7284020664887872E-3</v>
+      </c>
+      <c r="T9" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="U9" s="4">
+        <v>8.9050104018420246E-4</v>
+      </c>
+      <c r="V9" s="4">
+        <v>7.0182112751593449E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.94034876774283982</v>
+      </c>
+      <c r="E10" s="3">
+        <v>5.3256141378915798</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1.2006885021838241</v>
+      </c>
+      <c r="J10" s="3">
+        <v>4.1888637625061076</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="P10" s="4">
+        <v>1.024203187397551E-3</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>4.8706672985798947E-3</v>
+      </c>
+      <c r="T10" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="U10" s="4">
+        <v>8.7345378802373736E-4</v>
+      </c>
+      <c r="V10" s="4">
+        <v>8.8120279857618142E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1.0121474857262169</v>
+      </c>
+      <c r="E11" s="3">
+        <v>5.0935257716333666</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.97183873595508763</v>
+      </c>
+      <c r="J11" s="3">
+        <v>3.0411071567397259</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="P11" s="4">
+        <v>9.1429275878093168E-4</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>7.0963806581679232E-3</v>
+      </c>
+      <c r="T11" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="U11" s="4">
+        <v>9.5959056731180362E-4</v>
+      </c>
+      <c r="V11" s="4">
+        <v>5.8195493641756014E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.0215708125950289</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4.6239216862370558</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1.2320999977329381</v>
+      </c>
+      <c r="J12" s="3">
+        <v>2.5009803685037371</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="P12" s="4">
+        <v>9.0853039940785266E-4</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>6.2821065073317322E-3</v>
+      </c>
+      <c r="T12" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="U12" s="4">
+        <v>1.000602112469183E-3</v>
+      </c>
+      <c r="V12" s="4">
+        <v>4.6894207913342539E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.138917364969726</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3.9544372342178828</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.99656896141483953</v>
+      </c>
+      <c r="J13" s="3">
+        <v>3.9962800387399269</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="P13" s="4">
+        <v>9.8614330292833962E-4</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>6.0693554092539591E-3</v>
+      </c>
+      <c r="T13" s="2">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="U13" s="4">
+        <v>8.97539958757951E-4</v>
+      </c>
+      <c r="V13" s="4">
+        <v>7.210461423343072E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1.0570581444786731</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2.5812904422824481</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1.019499325510034</v>
+      </c>
+      <c r="J14" s="3">
+        <v>3.664944550156235</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="P14" s="4">
+        <v>9.6385088445594298E-4</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>5.1824056453252648E-3</v>
+      </c>
+      <c r="T14" s="2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="U14" s="4">
+        <v>9.3313014996185034E-4</v>
+      </c>
+      <c r="V14" s="4">
+        <v>6.6563622281744818E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1.2117980735284719</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1.677596723500917</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1.3102649020137871</v>
+      </c>
+      <c r="J15" s="3">
+        <v>2.372178744230395</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="P15" s="4">
+        <v>9.4568001951987645E-4</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>6.0509054619209924E-3</v>
+      </c>
+      <c r="T15" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="U15" s="4">
+        <v>9.2448569269220173E-4</v>
+      </c>
+      <c r="V15" s="4">
+        <v>5.5713613729078022E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1.5252678619409561</v>
+      </c>
+      <c r="E16" s="3">
+        <v>2.0949053100808008</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="I16" s="3">
+        <v>1.0838476724867809</v>
+      </c>
+      <c r="J16" s="3">
+        <v>4.0857824692155598</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="P16" s="4">
+        <v>9.1043045654642582E-4</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>6.4182455433808711E-3</v>
+      </c>
+      <c r="T16" s="2">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="U16" s="4">
+        <v>9.7813343192992342E-4</v>
+      </c>
+      <c r="V16" s="4">
+        <v>5.588069698938684E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1.1896217616969209</v>
+      </c>
+      <c r="E17" s="3">
+        <v>2.2609062125685142</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1.1662209653912841</v>
+      </c>
+      <c r="J17" s="3">
+        <v>4.7511562373955858</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="P17" s="4">
+        <v>9.2156286343361325E-4</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>6.5812898544779404E-3</v>
+      </c>
+      <c r="T17" s="2">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="U17" s="4">
+        <v>9.3864640250855124E-4</v>
+      </c>
+      <c r="V17" s="4">
+        <v>6.232337910902966E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1.3086360885859349</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1.851207611589089</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1.2219857534477061</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2.9975122792910991</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="P18" s="4">
+        <v>8.9859020429974054E-4</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>6.7538255888006269E-3</v>
+      </c>
+      <c r="T18" s="2">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="U18" s="4">
+        <v>8.1087155764451022E-4</v>
+      </c>
+      <c r="V18" s="4">
+        <v>8.1944715297911658E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1.077026451559286</v>
+      </c>
+      <c r="E19" s="3">
+        <v>4.1530368143786029</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I19" s="3">
+        <v>1.2036712213019161</v>
+      </c>
+      <c r="J19" s="3">
+        <v>2.5102127378794559</v>
+      </c>
+      <c r="O19" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="P19" s="4">
+        <v>9.2868146419403043E-4</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>7.7483937891313142E-3</v>
+      </c>
+      <c r="T19" s="2">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="U19" s="4">
+        <v>9.0590697593961379E-4</v>
+      </c>
+      <c r="V19" s="4">
+        <v>7.593555244641545E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1.356206693529314</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1.839396885268415</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1.013036824616053</v>
+      </c>
+      <c r="J20" s="3">
+        <v>3.016282088515001</v>
+      </c>
+      <c r="O20" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="P20" s="4">
+        <v>8.8140729833040407E-4</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>6.5942327828680076E-3</v>
+      </c>
+      <c r="T20" s="2">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="U20" s="4">
+        <v>9.0557647837213873E-4</v>
+      </c>
+      <c r="V20" s="4">
+        <v>7.5461846756831909E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1.1900963614755851</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2.187063856021787</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1.2624402615952719</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1.668337816377105</v>
+      </c>
+      <c r="O21" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="P21" s="4">
+        <v>9.6698191436237824E-4</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>6.7255155392929346E-3</v>
+      </c>
+      <c r="T21" s="2">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="U21" s="4">
+        <v>9.970750667908678E-4</v>
+      </c>
+      <c r="V21" s="4">
+        <v>4.7412430524547081E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1.08526160831916</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1.60004595633669</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I22" s="3">
+        <v>1.167505707045347</v>
+      </c>
+      <c r="J22" s="3">
+        <v>2.0810840606199812</v>
+      </c>
+      <c r="O22" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="P22" s="4">
+        <v>9.4260885795258696E-4</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>5.1189678753029806E-3</v>
+      </c>
+      <c r="T22" s="2">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="U22" s="4">
+        <v>8.8527316283143595E-4</v>
+      </c>
+      <c r="V22" s="4">
+        <v>7.3950155175083561E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.98063972528183418</v>
+      </c>
+      <c r="E23" s="3">
+        <v>4.0375333828575197</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I23" s="3">
+        <v>1.1753641102935319</v>
+      </c>
+      <c r="J23" s="3">
+        <v>2.5002450458435481</v>
+      </c>
+      <c r="O23" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="P23" s="4">
+        <v>9.477685169473946E-4</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>5.3796954279437953E-3</v>
+      </c>
+      <c r="T23" s="2">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="U23" s="4">
+        <v>8.7271559401397964E-4</v>
+      </c>
+      <c r="V23" s="4">
+        <v>6.4661265226357368E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1.247853113988759</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1.7883271602324831</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I24" s="3">
+        <v>1.09977429446077</v>
+      </c>
+      <c r="J24" s="3">
+        <v>2.2089143870114052</v>
+      </c>
+      <c r="O24" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="P24" s="4">
+        <v>9.1269067669933835E-4</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>6.3851591652298607E-3</v>
+      </c>
+      <c r="T24" s="2">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="U24" s="4">
+        <v>9.535531562039275E-4</v>
+      </c>
+      <c r="V24" s="4">
+        <v>5.265783078721299E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1.3026846083723591</v>
+      </c>
+      <c r="E25" s="3">
+        <v>2.7567520245772501</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0.93259443929884955</v>
+      </c>
+      <c r="J25" s="3">
+        <v>4.3556272388492827</v>
+      </c>
+      <c r="O25" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="P25" s="4">
+        <v>9.258629991388802E-4</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>6.4743543351801014E-3</v>
+      </c>
+      <c r="T25" s="2">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="U25" s="4">
+        <v>9.7794115955868177E-4</v>
+      </c>
+      <c r="V25" s="4">
+        <v>5.2613637433965516E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1.099241135447669</v>
+      </c>
+      <c r="E26" s="3">
+        <v>2.4795267418455089</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="I26" s="3">
+        <v>1.3141825053691081</v>
+      </c>
+      <c r="J26" s="3">
+        <v>3.564915048701697</v>
+      </c>
+      <c r="O26" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="P26" s="4">
+        <v>9.5619688271728889E-4</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>5.5360916209526417E-3</v>
+      </c>
+      <c r="T26" s="2">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="U26" s="4">
+        <v>9.0016825812679264E-4</v>
+      </c>
+      <c r="V26" s="4">
+        <v>6.2060187817966489E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1.285968036394874</v>
+      </c>
+      <c r="E27" s="3">
+        <v>3.121608480448121</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I27" s="3">
+        <v>1.3469689784515011</v>
+      </c>
+      <c r="J27" s="3">
+        <v>2.346437488938832</v>
+      </c>
+      <c r="O27" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="P27" s="4">
+        <v>9.2594755224886143E-4</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>6.1565018393133254E-3</v>
+      </c>
+      <c r="T27" s="2">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="U27" s="4">
+        <v>1.015241755845895E-3</v>
+      </c>
+      <c r="V27" s="4">
+        <v>4.4788025287490138E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1.1904958824152601</v>
+      </c>
+      <c r="E28" s="3">
+        <v>2.2181372187220778</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="I28" s="3">
+        <v>1.012095471690114</v>
+      </c>
+      <c r="J28" s="3">
+        <v>4.4413238911003941</v>
+      </c>
+      <c r="O28" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="P28" s="4">
+        <v>9.100966165375453E-4</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>6.9612827810649428E-3</v>
+      </c>
+      <c r="T28" s="2">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="U28" s="4">
+        <v>9.2899420333204493E-4</v>
+      </c>
+      <c r="V28" s="4">
+        <v>5.5947557613445836E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.8998473243361742</v>
+      </c>
+      <c r="E29" s="3">
+        <v>7.09467169486771</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1.065548328414299</v>
+      </c>
+      <c r="J29" s="3">
+        <v>3.336861284190475</v>
+      </c>
+      <c r="O29" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="P29" s="4">
+        <v>1.0049581263010881E-3</v>
+      </c>
+      <c r="Q29" s="4">
+        <v>5.4965965858551303E-3</v>
+      </c>
+      <c r="T29" s="2">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="U29" s="4">
+        <v>9.4393048004325661E-4</v>
+      </c>
+      <c r="V29" s="4">
+        <v>5.3743688896886153E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1.468253258723812</v>
+      </c>
+      <c r="E30" s="3">
+        <v>2.0598754398207682</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I30" s="3">
+        <v>1.110294805691481</v>
+      </c>
+      <c r="J30" s="3">
+        <v>2.683816720258009</v>
+      </c>
+      <c r="O30" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="P30" s="4">
+        <v>8.9695096154903016E-4</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>6.9720673775854397E-3</v>
+      </c>
+      <c r="T30" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="U30" s="4">
+        <v>7.7791704414868518E-4</v>
+      </c>
+      <c r="V30" s="4">
+        <v>1.0112245780850661E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1.2405468639603969</v>
+      </c>
+      <c r="E31" s="3">
+        <v>2.2424909217316151</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="I31" s="3">
+        <v>1.0535723534019239</v>
+      </c>
+      <c r="J31" s="3">
+        <v>3.57424997229566</v>
+      </c>
+      <c r="O31" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="P31" s="4">
+        <v>8.8400873760446008E-4</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>8.2958166378902989E-3</v>
+      </c>
+      <c r="T31" s="2">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="U31" s="4">
+        <v>8.1101238271637655E-4</v>
+      </c>
+      <c r="V31" s="4">
+        <v>9.3658771157432673E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1.320821067296722</v>
+      </c>
+      <c r="E32" s="3">
+        <v>2.608599231783272</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="I32" s="3">
+        <v>1.158579216995659</v>
+      </c>
+      <c r="J32" s="3">
+        <v>3.6601016134220861</v>
+      </c>
+      <c r="O32" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="P32" s="4">
+        <v>9.0128958056342242E-4</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>7.1706374914660732E-3</v>
+      </c>
+      <c r="T32" s="2">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="U32" s="4">
+        <v>1.0162481881235651E-3</v>
+      </c>
+      <c r="V32" s="4">
+        <v>6.8972753484131963E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1.2043568008466421</v>
+      </c>
+      <c r="E33" s="3">
+        <v>2.328319183134639</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="I33" s="3">
+        <v>0.84174423775773644</v>
+      </c>
+      <c r="J33" s="3">
+        <v>4.6999219255485656</v>
+      </c>
+      <c r="O33" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="P33" s="4">
+        <v>9.0912040693944126E-4</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>5.8064167310642777E-3</v>
+      </c>
+      <c r="T33" s="2">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="U33" s="4">
+        <v>9.3439847932420329E-4</v>
+      </c>
+      <c r="V33" s="4">
+        <v>6.3234373070772372E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1.1481534644030471</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1.9602978792595189</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="I34" s="3">
+        <v>1.0934008193345459</v>
+      </c>
+      <c r="J34" s="3">
+        <v>2.42164879516839</v>
+      </c>
+      <c r="O34" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="P34" s="4">
+        <v>1.023442241876263E-3</v>
+      </c>
+      <c r="Q34" s="4">
+        <v>5.9907821679922174E-3</v>
+      </c>
+      <c r="T34" s="2">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="U34" s="4">
+        <v>9.0069347789100741E-4</v>
+      </c>
+      <c r="V34" s="4">
+        <v>6.9893486861439952E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1.191427924979201</v>
+      </c>
+      <c r="E35" s="3">
+        <v>2.886479600721982</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I35" s="3">
+        <v>1.254868022178572</v>
+      </c>
+      <c r="J35" s="3">
+        <v>2.2680376523431041</v>
+      </c>
+      <c r="O35" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="P35" s="4">
+        <v>8.5309648114304806E-4</v>
+      </c>
+      <c r="Q35" s="4">
+        <v>6.7834253073832387E-3</v>
+      </c>
+      <c r="T35" s="2">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="U35" s="4">
+        <v>9.7227946116014159E-4</v>
+      </c>
+      <c r="V35" s="4">
+        <v>6.8224504642190997E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1.397398083734074</v>
+      </c>
+      <c r="E36" s="3">
+        <v>2.0370402508698948</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="I36" s="3">
+        <v>1.001082750529644</v>
+      </c>
+      <c r="J36" s="3">
+        <v>4.9595770297358257</v>
+      </c>
+      <c r="O36" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="P36" s="4">
+        <v>1.0193762250413571E-3</v>
+      </c>
+      <c r="Q36" s="4">
+        <v>5.2984692532484874E-3</v>
+      </c>
+      <c r="T36" s="2">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="U36" s="4">
+        <v>9.2384478130150564E-4</v>
+      </c>
+      <c r="V36" s="4">
+        <v>5.835685680643965E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1.063087104993955</v>
+      </c>
+      <c r="E37" s="3">
+        <v>2.7495281753048468</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="I37" s="3">
+        <v>1.046557641152625</v>
+      </c>
+      <c r="J37" s="3">
+        <v>2.668968520250568</v>
+      </c>
+      <c r="O37" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="P37" s="4">
+        <v>9.0432664910439112E-4</v>
+      </c>
+      <c r="Q37" s="4">
+        <v>7.0568925162746302E-3</v>
+      </c>
+      <c r="T37" s="2">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="U37" s="4">
+        <v>8.8436240981511953E-4</v>
+      </c>
+      <c r="V37" s="4">
+        <v>5.7945371857014462E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1.208349551353872</v>
+      </c>
+      <c r="E38" s="3">
+        <v>2.560692724154114</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="I38" s="3">
+        <v>1.110275789111471</v>
+      </c>
+      <c r="J38" s="3">
+        <v>4.2630630981432596</v>
+      </c>
+      <c r="O38" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="P38" s="4">
+        <v>1.0051419302351801E-3</v>
+      </c>
+      <c r="Q38" s="4">
+        <v>5.0788481511067751E-3</v>
+      </c>
+      <c r="T38" s="2">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="U38" s="4">
+        <v>8.8315389679396485E-4</v>
+      </c>
+      <c r="V38" s="4">
+        <v>5.1902964772459472E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1.0376609122206899</v>
+      </c>
+      <c r="E39" s="3">
+        <v>3.5619617170987632</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="I39" s="3">
+        <v>1.250792391554042</v>
+      </c>
+      <c r="J39" s="3">
+        <v>2.1990918293919011</v>
+      </c>
+      <c r="O39" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="P39" s="4">
+        <v>1.0192120170008749E-3</v>
+      </c>
+      <c r="Q39" s="4">
+        <v>4.2855002135541798E-3</v>
+      </c>
+      <c r="T39" s="2">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="U39" s="4">
+        <v>9.4052651053605832E-4</v>
+      </c>
+      <c r="V39" s="4">
+        <v>6.4219400244938246E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1.347269213052021</v>
+      </c>
+      <c r="E40" s="3">
+        <v>2.4589019659816072</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="I40" s="3">
+        <v>1.173786659870979</v>
+      </c>
+      <c r="J40" s="3">
+        <v>3.518310711451949</v>
+      </c>
+      <c r="O40" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="P40" s="4">
+        <v>9.2208933522913738E-4</v>
+      </c>
+      <c r="Q40" s="4">
+        <v>5.7291648913626574E-3</v>
+      </c>
+      <c r="T40" s="2">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="U40" s="4">
+        <v>8.1209128390349677E-4</v>
+      </c>
+      <c r="V40" s="4">
+        <v>8.2393522462164675E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1.08397405059351</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1.867224051310461</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="I41" s="3">
+        <v>1.187407037000862</v>
+      </c>
+      <c r="J41" s="3">
+        <v>4.45654008861999</v>
+      </c>
+      <c r="O41" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="P41" s="4">
+        <v>9.3217466591216278E-4</v>
+      </c>
+      <c r="Q41" s="4">
+        <v>7.3628738334350656E-3</v>
+      </c>
+      <c r="T41" s="2">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="U41" s="4">
+        <v>8.7365716151930164E-4</v>
+      </c>
+      <c r="V41" s="4">
+        <v>6.052312985222361E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1.1673806908197391</v>
+      </c>
+      <c r="E42" s="3">
+        <v>2.16408464525334</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="I42" s="3">
+        <v>1.424038306492494</v>
+      </c>
+      <c r="J42" s="3">
+        <v>2.057732905258264</v>
+      </c>
+      <c r="O42" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="P42" s="4">
+        <v>9.0407840970345627E-4</v>
+      </c>
+      <c r="Q42" s="4">
+        <v>7.7768923523061934E-3</v>
+      </c>
+      <c r="T42" s="2">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="U42" s="4">
+        <v>9.1587946043700783E-4</v>
+      </c>
+      <c r="V42" s="4">
+        <v>5.2451061850339051E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1.1131675225327931</v>
+      </c>
+      <c r="E43" s="3">
+        <v>3.0341103181973459</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="I43" s="3">
+        <v>1.1814852334795909</v>
+      </c>
+      <c r="J43" s="3">
+        <v>2.1799403207238379</v>
+      </c>
+      <c r="O43" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="P43" s="4">
+        <v>9.5436819020081032E-4</v>
+      </c>
+      <c r="Q43" s="4">
+        <v>5.8898190330647091E-3</v>
+      </c>
+      <c r="T43" s="2">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="U43" s="4">
+        <v>8.9343627504547311E-4</v>
+      </c>
+      <c r="V43" s="4">
+        <v>5.8037782182251479E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D44" s="3">
+        <v>1.317787310340967</v>
+      </c>
+      <c r="E44" s="3">
+        <v>1.9015016274806491</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="I44" s="3">
+        <v>1.1745862018380411</v>
+      </c>
+      <c r="J44" s="3">
+        <v>3.5024018465791982</v>
+      </c>
+      <c r="O44" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="P44" s="4">
+        <v>9.3836815697840421E-4</v>
+      </c>
+      <c r="Q44" s="4">
+        <v>6.6703860002955209E-3</v>
+      </c>
+      <c r="T44" s="2">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="U44" s="4">
+        <v>9.7551464150883176E-4</v>
+      </c>
+      <c r="V44" s="4">
+        <v>6.2514298095603044E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0.85357227491798637</v>
+      </c>
+      <c r="E45" s="3">
+        <v>6.7284237569665981</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="I45" s="3">
+        <v>1.2575616808069101</v>
+      </c>
+      <c r="J45" s="3">
+        <v>2.3695625838051382</v>
+      </c>
+      <c r="O45" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="P45" s="4">
+        <v>9.7553804657307924E-4</v>
+      </c>
+      <c r="Q45" s="4">
+        <v>5.8993855345631924E-3</v>
+      </c>
+      <c r="T45" s="2">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="U45" s="4">
+        <v>8.4771113559812129E-4</v>
+      </c>
+      <c r="V45" s="4">
+        <v>8.3069433673470718E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1.2667193803499599</v>
+      </c>
+      <c r="E46" s="3">
+        <v>2.5562570431765161</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="I46" s="3">
+        <v>1.488035409056041</v>
+      </c>
+      <c r="J46" s="3">
+        <v>1.921014030674268</v>
+      </c>
+      <c r="O46" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="P46" s="4">
+        <v>9.0317000385979715E-4</v>
+      </c>
+      <c r="Q46" s="4">
+        <v>7.8804752263929145E-3</v>
+      </c>
+      <c r="T46" s="2">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="U46" s="4">
+        <v>8.781766987495433E-4</v>
+      </c>
+      <c r="V46" s="4">
+        <v>6.53197148873741E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1.2665557089188391</v>
+      </c>
+      <c r="E47" s="3">
+        <v>2.3333529682993772</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="I47" s="3">
+        <v>1.2551492704235729</v>
+      </c>
+      <c r="J47" s="3">
+        <v>1.4937996371929949</v>
+      </c>
+      <c r="O47" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="P47" s="4">
+        <v>9.3899192033260962E-4</v>
+      </c>
+      <c r="Q47" s="4">
+        <v>7.5755984248804297E-3</v>
+      </c>
+      <c r="T47" s="2">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="U47" s="4">
+        <v>8.9820920089064729E-4</v>
+      </c>
+      <c r="V47" s="4">
+        <v>7.4229273020972814E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1.1362498679997659</v>
+      </c>
+      <c r="E48" s="3">
+        <v>2.5732707697016921</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="I48" s="3">
+        <v>1.100267778188835</v>
+      </c>
+      <c r="J48" s="3">
+        <v>3.2564510473139658</v>
+      </c>
+      <c r="O48" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="P48" s="4">
+        <v>8.9660596251005514E-4</v>
+      </c>
+      <c r="Q48" s="4">
+        <v>7.4475466774189224E-3</v>
+      </c>
+      <c r="T48" s="2">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="U48" s="4">
+        <v>9.0615864008485503E-4</v>
+      </c>
+      <c r="V48" s="4">
+        <v>5.9616225295558217E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D49" s="3">
+        <v>1.043925586311016</v>
+      </c>
+      <c r="E49" s="3">
+        <v>2.9588101316047331</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="I49" s="3">
+        <v>0.89387874112959853</v>
+      </c>
+      <c r="J49" s="3">
+        <v>5.5259222926915719</v>
+      </c>
+      <c r="O49" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="P49" s="4">
+        <v>9.332544949627611E-4</v>
+      </c>
+      <c r="Q49" s="4">
+        <v>5.5164065201718671E-3</v>
+      </c>
+      <c r="T49" s="2">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="U49" s="4">
+        <v>8.951977412125368E-4</v>
+      </c>
+      <c r="V49" s="4">
+        <v>6.2963024719676257E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1.1640722779636701</v>
+      </c>
+      <c r="E50" s="3">
+        <v>3.1516746441330592</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="I50" s="3">
+        <v>1.1678838326836289</v>
+      </c>
+      <c r="J50" s="3">
+        <v>2.3319695451395588</v>
+      </c>
+      <c r="O50" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="P50" s="4">
+        <v>8.9297855997397539E-4</v>
+      </c>
+      <c r="Q50" s="4">
+        <v>7.9149877342538956E-3</v>
+      </c>
+      <c r="T50" s="2">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="U50" s="4">
+        <v>8.354892445129609E-4</v>
+      </c>
+      <c r="V50" s="4">
+        <v>7.7759996260347809E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D51" s="3">
+        <v>1.12677083333433</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1.876406953901137</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="I51" s="3">
+        <v>0.85335667574715135</v>
+      </c>
+      <c r="J51" s="3">
+        <v>4.8235040520135648</v>
+      </c>
+      <c r="O51" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="P51" s="4">
+        <v>9.5206427351085781E-4</v>
+      </c>
+      <c r="Q51" s="4">
+        <v>5.239649765037083E-3</v>
+      </c>
+      <c r="T51" s="2">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="U51" s="4">
+        <v>9.9070051289274863E-4</v>
+      </c>
+      <c r="V51" s="4">
+        <v>4.8704509442503516E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0.88592487970189449</v>
+      </c>
+      <c r="E52" s="3">
+        <v>6.5971396548057202</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="I52" s="3">
+        <v>1.3214190617321111</v>
+      </c>
+      <c r="J52" s="3">
+        <v>3.481882612508719</v>
+      </c>
+      <c r="O52" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="P52" s="4">
+        <v>9.2519791373159061E-4</v>
+      </c>
+      <c r="Q52" s="4">
+        <v>5.1244136787218604E-3</v>
+      </c>
+      <c r="T52" s="2">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="U52" s="4">
+        <v>8.1560905800920152E-4</v>
+      </c>
+      <c r="V52" s="4">
+        <v>7.5256056845682869E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D53" s="3">
+        <v>1.1628513982455959</v>
+      </c>
+      <c r="E53" s="3">
+        <v>2.263982885489348</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="I53" s="3">
+        <v>1.093655591018923</v>
+      </c>
+      <c r="J53" s="3">
+        <v>1.8501222996397351</v>
+      </c>
+      <c r="O53" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="P53" s="4">
+        <v>9.2016083846492146E-4</v>
+      </c>
+      <c r="Q53" s="4">
+        <v>6.3130335886868953E-3</v>
+      </c>
+      <c r="T53" s="2">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="U53" s="4">
+        <v>7.6591156694121021E-4</v>
+      </c>
+      <c r="V53" s="4">
+        <v>1.248598281393873E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D54" s="3">
+        <v>1.3763428007271949</v>
+      </c>
+      <c r="E54" s="3">
+        <v>2.3741232428182348</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="I54" s="3">
+        <v>1.3146897790882119</v>
+      </c>
+      <c r="J54" s="3">
+        <v>1.482013962253355</v>
+      </c>
+      <c r="O54" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="P54" s="4">
+        <v>9.2929885570699491E-4</v>
+      </c>
+      <c r="Q54" s="4">
+        <v>6.5689869800932546E-3</v>
+      </c>
+      <c r="T54" s="2">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="U54" s="4">
+        <v>8.7947686879334371E-4</v>
+      </c>
+      <c r="V54" s="4">
+        <v>7.0561020580377802E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C55" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D55" s="3">
+        <v>1.274361759814852</v>
+      </c>
+      <c r="E55" s="3">
+        <v>2.9399033213789258</v>
+      </c>
+      <c r="H55" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I55" s="3">
+        <v>1.248787802058223</v>
+      </c>
+      <c r="J55" s="3">
+        <v>2.1981989245154052</v>
+      </c>
+      <c r="O55" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="P55" s="4">
+        <v>9.4848740831921094E-4</v>
+      </c>
+      <c r="Q55" s="4">
+        <v>6.0143025932583964E-3</v>
+      </c>
+      <c r="T55" s="2">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="U55" s="4">
+        <v>9.8520832375428337E-4</v>
+      </c>
+      <c r="V55" s="4">
+        <v>6.1705349126849919E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="3">
+        <f>AVERAGE(D6:D55)</f>
+        <v>1.1689923572027021</v>
+      </c>
+      <c r="E57" s="3">
+        <f>AVERAGE(E6:E55)</f>
+        <v>2.9724080693133152</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I57" s="3">
+        <f>AVERAGE(I6:I55)</f>
+        <v>1.1537411407047635</v>
+      </c>
+      <c r="J57" s="3">
+        <f>AVERAGE(J6:J55)</f>
+        <v>3.0832685520458192</v>
+      </c>
+      <c r="O57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P57" s="4">
+        <f>AVERAGE(P6:P55)</f>
+        <v>9.3433744070495108E-4</v>
+      </c>
+      <c r="Q57" s="4">
+        <f>AVERAGE(Q6:Q55)</f>
+        <v>6.4097520900457759E-3</v>
+      </c>
+      <c r="T57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U57" s="4">
+        <f>AVERAGE(U6:U55)</f>
+        <v>9.1146276647322694E-4</v>
+      </c>
+      <c r="V57" s="4">
+        <f>AVERAGE(V6:V55)</f>
+        <v>6.6134327801047142E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="3">
+        <f>_xlfn.STDEV.S(D6:D55)</f>
+        <v>0.14528175160352255</v>
+      </c>
+      <c r="E58" s="3">
+        <f>_xlfn.STDEV.S(E6:E55)</f>
+        <v>1.3111645875663389</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I58" s="3">
+        <f>_xlfn.STDEV.S(I6:I55)</f>
+        <v>0.14381506205316286</v>
+      </c>
+      <c r="J58" s="3">
+        <f>_xlfn.STDEV.S(J6:J55)</f>
+        <v>1.0508976860221078</v>
+      </c>
+      <c r="O58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P58" s="4">
+        <f>_xlfn.STDEV.S(P6:P55)</f>
+        <v>4.2054007790966928E-5</v>
+      </c>
+      <c r="Q58" s="4">
+        <f>_xlfn.STDEV.S(Q6:Q55)</f>
+        <v>9.4829231983438152E-4</v>
+      </c>
+      <c r="T58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="U58" s="4">
+        <f>_xlfn.STDEV.S(U6:U55)</f>
+        <v>6.0997195610198861E-5</v>
+      </c>
+      <c r="V58" s="4">
+        <f>_xlfn.STDEV.S(V6:V55)</f>
+        <v>1.4796067294317152E-3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -409,7 +2684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:T58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Test-8 for tree (nextyear, mse&mape)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-7.xlsx
+++ b/migforecasting/underground/test-7.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="16">
   <si>
     <t>test size 20%</t>
   </si>
@@ -58,12 +58,6 @@
     <t>Random Forest-100 (citiesdataset-DCor-3.csv) - this year</t>
   </si>
   <si>
-    <t>Random Forest-100 (citiesdataset-NYDcor-2.csv) - this year</t>
-  </si>
-  <si>
-    <t>Random Forest-100 (citiesdataset-NYDCor-3.csv) - this year</t>
-  </si>
-  <si>
     <t>test 20%</t>
   </si>
   <si>
@@ -71,6 +65,9 @@
   </si>
   <si>
     <t>NN(64,64,64,64,1) (citiesdataset-NYDcor-3.csv) - next year</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (citiesdataset-Dcor-2.csv) - this year</t>
   </si>
 </sst>
 </file>
@@ -422,7 +419,7 @@
   <dimension ref="C3:V121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,11 +458,11 @@
       </c>
       <c r="J4" s="1"/>
       <c r="O4" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="T4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="V4" s="1"/>
     </row>
@@ -3164,10 +3161,10 @@
         <v>0</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="3:31" x14ac:dyDescent="0.25">
@@ -3188,10 +3185,10 @@
       </c>
       <c r="T4" s="1"/>
       <c r="X4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="3:31" x14ac:dyDescent="0.25">

</xml_diff>